<commit_message>
Ajustes en primera pasada
Se tenia el remplzao de los iden por los tipos antes de que se tuvieran todos los tipos
</commit_message>
<xml_diff>
--- a/Quindim/Quindim Src.xlsx
+++ b/Quindim/Quindim Src.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITNL\7° Semestre - I.S.C\Leng. y Automat. 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arman\Documents\ITNL\7mo Semestre\Lenguajes y Automatas II\Quindim\AnalizadorLexico\Quindim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC68D5A-0C5B-4350-9334-2BC648EF3DED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5ADA1B8-BF45-45FE-AA7B-08F708AC4081}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{674D8D03-4B2E-43D7-B73B-FEE82AEA8288}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{674D8D03-4B2E-43D7-B73B-FEE82AEA8288}"/>
   </bookViews>
   <sheets>
     <sheet name="Lexicon" sheetId="1" r:id="rId1"/>
     <sheet name="Grammar" sheetId="3" r:id="rId2"/>
-    <sheet name="Examples Syntax" sheetId="2" r:id="rId3"/>
+    <sheet name="Semantic Rules" sheetId="4" r:id="rId3"/>
+    <sheet name="Examples Syntax" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="259">
   <si>
     <t>print</t>
   </si>
@@ -776,13 +777,46 @@
   </si>
   <si>
     <t>Right Side</t>
+  </si>
+  <si>
+    <t>Quindim Semantic</t>
+  </si>
+  <si>
+    <t>TDD1 INTE</t>
+  </si>
+  <si>
+    <t>TDD2 DBLE</t>
+  </si>
+  <si>
+    <t>TDD3 CHAR</t>
+  </si>
+  <si>
+    <t>TDD4 STRG</t>
+  </si>
+  <si>
+    <t>PR13 INTE</t>
+  </si>
+  <si>
+    <t>PR13 DBLE</t>
+  </si>
+  <si>
+    <t>PR13 CHAR</t>
+  </si>
+  <si>
+    <t>PR13 STRG</t>
+  </si>
+  <si>
+    <t>INTE</t>
+  </si>
+  <si>
+    <t>DBLE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -847,7 +881,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -869,8 +903,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -880,15 +926,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1013,6 +1050,56 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="711477" cy="721905"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{228F3172-6069-4FE1-86D3-D62EDA1C63B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="57150" y="0"/>
+          <a:ext cx="711477" cy="721905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -1365,24 +1452,24 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="3" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:5" ht="73.150000000000006" customHeight="1">
+      <c r="A1" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
         <v>63</v>
       </c>
@@ -1399,7 +1486,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="7" t="s">
         <v>64</v>
       </c>
@@ -1416,7 +1503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
         <v>65</v>
       </c>
@@ -1433,7 +1520,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" s="7" t="s">
         <v>66</v>
       </c>
@@ -1450,7 +1537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" s="7" t="s">
         <v>67</v>
       </c>
@@ -1467,7 +1554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="7" t="s">
         <v>68</v>
       </c>
@@ -1484,7 +1571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="7" t="s">
         <v>69</v>
       </c>
@@ -1501,7 +1588,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="7" t="s">
         <v>70</v>
       </c>
@@ -1518,7 +1605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="7" t="s">
         <v>71</v>
       </c>
@@ -1535,7 +1622,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" s="7" t="s">
         <v>72</v>
       </c>
@@ -1552,7 +1639,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="7" t="s">
         <v>73</v>
       </c>
@@ -1569,7 +1656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" s="7" t="s">
         <v>74</v>
       </c>
@@ -1584,7 +1671,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" s="7" t="s">
         <v>75</v>
       </c>
@@ -1599,7 +1686,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" s="7" t="s">
         <v>76</v>
       </c>
@@ -1614,7 +1701,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" s="7" t="s">
         <v>77</v>
       </c>
@@ -1629,7 +1716,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5">
       <c r="A17" s="7" t="s">
         <v>78</v>
       </c>
@@ -1644,7 +1731,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5">
       <c r="A18" s="7" t="s">
         <v>79</v>
       </c>
@@ -1656,7 +1743,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5">
       <c r="A19" s="7" t="s">
         <v>80</v>
       </c>
@@ -1665,7 +1752,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5">
       <c r="A20" s="7" t="s">
         <v>81</v>
       </c>
@@ -1674,7 +1761,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5">
       <c r="A21" s="7" t="s">
         <v>82</v>
       </c>
@@ -1683,7 +1770,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
         <v>83</v>
       </c>
@@ -1692,7 +1779,7 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
         <v>84</v>
       </c>
@@ -1701,7 +1788,7 @@
       </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5">
       <c r="A24" s="7" t="s">
         <v>85</v>
       </c>
@@ -1710,7 +1797,7 @@
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5">
       <c r="A25" s="7" t="s">
         <v>86</v>
       </c>
@@ -1719,23 +1806,23 @@
       </c>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5">
       <c r="B26" s="4"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5">
       <c r="E27" s="4"/>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:3">
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3">
       <c r="C49" s="3"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:3">
       <c r="B57" s="3"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:3">
       <c r="B58" s="3"/>
     </row>
   </sheetData>
@@ -1752,26 +1839,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2903DA20-C73D-46F2-9130-B4272A66A295}">
   <dimension ref="A1:C148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="A144" workbookViewId="0">
+      <selection activeCell="H156" sqref="H156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" customWidth="1"/>
-    <col min="2" max="2" width="51.109375" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:3" ht="59.45" customHeight="1">
+      <c r="A1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="15"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B1" s="12"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
         <v>246</v>
       </c>
@@ -1779,7 +1866,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="8" t="s">
         <v>106</v>
       </c>
@@ -1787,7 +1874,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="8" t="s">
         <v>108</v>
       </c>
@@ -1795,7 +1882,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="8" t="s">
         <v>109</v>
       </c>
@@ -1803,7 +1890,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="8" t="s">
         <v>109</v>
       </c>
@@ -1811,7 +1898,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="8" t="s">
         <v>109</v>
       </c>
@@ -1819,7 +1906,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="8" t="s">
         <v>109</v>
       </c>
@@ -1827,7 +1914,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="8" t="s">
         <v>109</v>
       </c>
@@ -1835,7 +1922,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" s="8" t="s">
         <v>109</v>
       </c>
@@ -1843,7 +1930,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="8" t="s">
         <v>109</v>
       </c>
@@ -1851,7 +1938,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" s="8" t="s">
         <v>109</v>
       </c>
@@ -1859,7 +1946,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="8" t="s">
         <v>109</v>
       </c>
@@ -1867,7 +1954,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="8" t="s">
         <v>109</v>
       </c>
@@ -1875,7 +1962,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="8" t="s">
         <v>109</v>
       </c>
@@ -1883,7 +1970,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" s="8" t="s">
         <v>109</v>
       </c>
@@ -1891,7 +1978,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2">
       <c r="A17" s="8" t="s">
         <v>109</v>
       </c>
@@ -1899,7 +1986,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2">
       <c r="A18" s="8" t="s">
         <v>111</v>
       </c>
@@ -1907,7 +1994,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2">
       <c r="A19" s="8" t="s">
         <v>117</v>
       </c>
@@ -1915,7 +2002,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2">
       <c r="A20" s="8" t="s">
         <v>117</v>
       </c>
@@ -1923,7 +2010,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2">
       <c r="A21" s="8" t="s">
         <v>117</v>
       </c>
@@ -1931,7 +2018,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2">
       <c r="A22" s="8" t="s">
         <v>117</v>
       </c>
@@ -1939,7 +2026,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2">
       <c r="A23" s="8" t="s">
         <v>117</v>
       </c>
@@ -1947,7 +2034,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2">
       <c r="A24" s="8" t="s">
         <v>117</v>
       </c>
@@ -1955,7 +2042,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2">
       <c r="A25" s="8" t="s">
         <v>117</v>
       </c>
@@ -1963,7 +2050,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2">
       <c r="A26" s="8" t="s">
         <v>130</v>
       </c>
@@ -1971,7 +2058,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2">
       <c r="A27" s="8" t="s">
         <v>130</v>
       </c>
@@ -1979,7 +2066,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2">
       <c r="A28" s="8" t="s">
         <v>130</v>
       </c>
@@ -1987,7 +2074,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2">
       <c r="A29" s="8" t="s">
         <v>130</v>
       </c>
@@ -1995,7 +2082,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2">
       <c r="A30" s="8" t="s">
         <v>130</v>
       </c>
@@ -2003,7 +2090,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2">
       <c r="A31" s="8" t="s">
         <v>130</v>
       </c>
@@ -2011,7 +2098,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2">
       <c r="A32" s="8" t="s">
         <v>130</v>
       </c>
@@ -2019,7 +2106,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2">
       <c r="A33" s="8" t="s">
         <v>130</v>
       </c>
@@ -2027,7 +2114,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2">
       <c r="A34" s="8" t="s">
         <v>130</v>
       </c>
@@ -2035,7 +2122,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2">
       <c r="A35" s="8" t="s">
         <v>130</v>
       </c>
@@ -2043,7 +2130,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2">
       <c r="A36" s="8" t="s">
         <v>130</v>
       </c>
@@ -2051,7 +2138,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2">
       <c r="A37" s="8" t="s">
         <v>108</v>
       </c>
@@ -2059,7 +2146,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2">
       <c r="A38" s="8" t="s">
         <v>108</v>
       </c>
@@ -2067,7 +2154,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2">
       <c r="A39" s="8" t="s">
         <v>108</v>
       </c>
@@ -2075,7 +2162,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2">
       <c r="A40" s="8" t="s">
         <v>108</v>
       </c>
@@ -2083,7 +2170,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2">
       <c r="A41" s="8" t="s">
         <v>146</v>
       </c>
@@ -2091,7 +2178,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2">
       <c r="A42" s="8" t="s">
         <v>146</v>
       </c>
@@ -2099,7 +2186,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2">
       <c r="A43" s="8" t="s">
         <v>146</v>
       </c>
@@ -2107,7 +2194,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2">
       <c r="A44" s="8" t="s">
         <v>146</v>
       </c>
@@ -2115,7 +2202,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2">
       <c r="A45" s="8" t="s">
         <v>118</v>
       </c>
@@ -2123,7 +2210,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2">
       <c r="A46" s="8" t="s">
         <v>118</v>
       </c>
@@ -2131,7 +2218,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2">
       <c r="A47" s="8" t="s">
         <v>114</v>
       </c>
@@ -2139,7 +2226,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2">
       <c r="A48" s="8" t="s">
         <v>114</v>
       </c>
@@ -2147,7 +2234,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2">
       <c r="A49" s="8" t="s">
         <v>114</v>
       </c>
@@ -2155,7 +2242,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2">
       <c r="A50" s="8" t="s">
         <v>114</v>
       </c>
@@ -2163,7 +2250,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2">
       <c r="A51" s="8" t="s">
         <v>114</v>
       </c>
@@ -2171,7 +2258,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2">
       <c r="A52" s="8" t="s">
         <v>114</v>
       </c>
@@ -2179,7 +2266,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2">
       <c r="A53" s="8" t="s">
         <v>112</v>
       </c>
@@ -2187,7 +2274,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2">
       <c r="A54" s="8" t="s">
         <v>112</v>
       </c>
@@ -2195,7 +2282,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2">
       <c r="A55" s="8" t="s">
         <v>112</v>
       </c>
@@ -2203,7 +2290,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2">
       <c r="A56" s="8" t="s">
         <v>112</v>
       </c>
@@ -2211,7 +2298,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2">
       <c r="A57" s="8" t="s">
         <v>163</v>
       </c>
@@ -2219,7 +2306,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2">
       <c r="A58" s="8" t="s">
         <v>163</v>
       </c>
@@ -2227,7 +2314,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2">
       <c r="A59" s="8" t="s">
         <v>109</v>
       </c>
@@ -2235,7 +2322,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2">
       <c r="A60" s="8" t="s">
         <v>163</v>
       </c>
@@ -2243,7 +2330,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2">
       <c r="A61" s="8" t="s">
         <v>166</v>
       </c>
@@ -2251,7 +2338,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2">
       <c r="A62" s="8" t="s">
         <v>166</v>
       </c>
@@ -2259,7 +2346,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2">
       <c r="A63" s="8" t="s">
         <v>166</v>
       </c>
@@ -2267,7 +2354,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2">
       <c r="A64" s="8" t="s">
         <v>166</v>
       </c>
@@ -2275,7 +2362,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2">
       <c r="A65" s="8" t="s">
         <v>166</v>
       </c>
@@ -2283,7 +2370,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2">
       <c r="A66" s="8" t="s">
         <v>113</v>
       </c>
@@ -2291,7 +2378,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2">
       <c r="A67" s="8" t="s">
         <v>113</v>
       </c>
@@ -2299,7 +2386,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2">
       <c r="A68" s="8" t="s">
         <v>115</v>
       </c>
@@ -2307,7 +2394,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2">
       <c r="A69" s="8" t="s">
         <v>175</v>
       </c>
@@ -2315,7 +2402,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2">
       <c r="A70" s="8" t="s">
         <v>175</v>
       </c>
@@ -2323,7 +2410,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2">
       <c r="A71" s="8" t="s">
         <v>176</v>
       </c>
@@ -2331,7 +2418,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2">
       <c r="A72" s="8" t="s">
         <v>176</v>
       </c>
@@ -2339,7 +2426,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2">
       <c r="A73" s="8" t="s">
         <v>176</v>
       </c>
@@ -2347,7 +2434,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2">
       <c r="A74" s="8" t="s">
         <v>176</v>
       </c>
@@ -2355,7 +2442,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2">
       <c r="A75" s="8" t="s">
         <v>178</v>
       </c>
@@ -2363,7 +2450,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2">
       <c r="A76" s="8" t="s">
         <v>178</v>
       </c>
@@ -2371,7 +2458,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2">
       <c r="A77" s="8" t="s">
         <v>178</v>
       </c>
@@ -2379,7 +2466,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2">
       <c r="A78" s="8" t="s">
         <v>178</v>
       </c>
@@ -2387,7 +2474,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2">
       <c r="A79" s="8" t="s">
         <v>178</v>
       </c>
@@ -2395,7 +2482,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2">
       <c r="A80" s="8" t="s">
         <v>178</v>
       </c>
@@ -2403,7 +2490,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2">
       <c r="A81" s="8" t="s">
         <v>185</v>
       </c>
@@ -2411,7 +2498,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2">
       <c r="A82" s="8" t="s">
         <v>187</v>
       </c>
@@ -2419,7 +2506,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2">
       <c r="A83" s="8" t="s">
         <v>187</v>
       </c>
@@ -2427,7 +2514,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2">
       <c r="A84" s="8" t="s">
         <v>187</v>
       </c>
@@ -2435,7 +2522,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2">
       <c r="A85" s="8" t="s">
         <v>187</v>
       </c>
@@ -2443,7 +2530,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2">
       <c r="A86" s="8" t="s">
         <v>191</v>
       </c>
@@ -2451,7 +2538,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2">
       <c r="A87" s="8" t="s">
         <v>191</v>
       </c>
@@ -2459,7 +2546,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2">
       <c r="A88" s="8" t="s">
         <v>191</v>
       </c>
@@ -2467,7 +2554,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2">
       <c r="A89" s="8" t="s">
         <v>191</v>
       </c>
@@ -2475,7 +2562,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2">
       <c r="A90" s="8" t="s">
         <v>191</v>
       </c>
@@ -2483,7 +2570,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2">
       <c r="A91" s="8" t="s">
         <v>193</v>
       </c>
@@ -2491,7 +2578,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2">
       <c r="A92" s="8" t="s">
         <v>194</v>
       </c>
@@ -2499,7 +2586,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2">
       <c r="A93" s="8" t="s">
         <v>194</v>
       </c>
@@ -2507,7 +2594,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2">
       <c r="A94" s="8" t="s">
         <v>194</v>
       </c>
@@ -2515,7 +2602,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2">
       <c r="A95" s="8" t="s">
         <v>119</v>
       </c>
@@ -2523,7 +2610,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2">
       <c r="A96" s="8" t="s">
         <v>119</v>
       </c>
@@ -2531,7 +2618,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2">
       <c r="A97" s="8" t="s">
         <v>195</v>
       </c>
@@ -2539,7 +2626,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2">
       <c r="A98" s="8" t="s">
         <v>195</v>
       </c>
@@ -2547,7 +2634,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2">
       <c r="A99" s="8" t="s">
         <v>195</v>
       </c>
@@ -2555,7 +2642,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2">
       <c r="A100" s="8" t="s">
         <v>195</v>
       </c>
@@ -2563,7 +2650,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2">
       <c r="A101" s="8" t="s">
         <v>195</v>
       </c>
@@ -2571,7 +2658,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2">
       <c r="A102" s="8" t="s">
         <v>195</v>
       </c>
@@ -2579,7 +2666,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2">
       <c r="A103" s="8" t="s">
         <v>195</v>
       </c>
@@ -2587,7 +2674,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2">
       <c r="A104" s="8" t="s">
         <v>195</v>
       </c>
@@ -2595,7 +2682,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2">
       <c r="A105" s="8" t="s">
         <v>195</v>
       </c>
@@ -2603,7 +2690,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2">
       <c r="A106" s="8" t="s">
         <v>195</v>
       </c>
@@ -2611,7 +2698,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2">
       <c r="A107" s="8" t="s">
         <v>195</v>
       </c>
@@ -2619,7 +2706,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2">
       <c r="A108" s="8" t="s">
         <v>195</v>
       </c>
@@ -2627,7 +2714,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2">
       <c r="A109" s="8" t="s">
         <v>211</v>
       </c>
@@ -2635,7 +2722,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2">
       <c r="A110" s="8" t="s">
         <v>211</v>
       </c>
@@ -2643,7 +2730,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2">
       <c r="A111" s="8" t="s">
         <v>211</v>
       </c>
@@ -2651,7 +2738,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2">
       <c r="A112" s="8" t="s">
         <v>211</v>
       </c>
@@ -2659,7 +2746,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2">
       <c r="A113" s="8" t="s">
         <v>211</v>
       </c>
@@ -2667,7 +2754,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2">
       <c r="A114" s="8" t="s">
         <v>211</v>
       </c>
@@ -2675,7 +2762,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2">
       <c r="A115" s="8" t="s">
         <v>211</v>
       </c>
@@ -2683,7 +2770,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2">
       <c r="A116" s="8" t="s">
         <v>211</v>
       </c>
@@ -2691,7 +2778,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2">
       <c r="A117" s="8" t="s">
         <v>211</v>
       </c>
@@ -2699,7 +2786,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2">
       <c r="A118" s="8" t="s">
         <v>211</v>
       </c>
@@ -2707,7 +2794,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2">
       <c r="A119" s="8" t="s">
         <v>211</v>
       </c>
@@ -2715,7 +2802,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2">
       <c r="A120" s="8" t="s">
         <v>222</v>
       </c>
@@ -2723,7 +2810,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2">
       <c r="A121" s="8" t="s">
         <v>222</v>
       </c>
@@ -2731,7 +2818,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2">
       <c r="A122" s="8" t="s">
         <v>222</v>
       </c>
@@ -2739,7 +2826,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2">
       <c r="A123" s="8" t="s">
         <v>222</v>
       </c>
@@ -2747,7 +2834,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2">
       <c r="A124" s="8" t="s">
         <v>222</v>
       </c>
@@ -2755,7 +2842,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2">
       <c r="A125" s="8" t="s">
         <v>222</v>
       </c>
@@ -2763,7 +2850,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2">
       <c r="A126" s="8" t="s">
         <v>109</v>
       </c>
@@ -2771,7 +2858,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2">
       <c r="A127" s="8" t="s">
         <v>120</v>
       </c>
@@ -2779,7 +2866,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2">
       <c r="A128" s="8" t="s">
         <v>120</v>
       </c>
@@ -2787,7 +2874,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2">
       <c r="A129" s="8" t="s">
         <v>120</v>
       </c>
@@ -2795,7 +2882,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2">
       <c r="A130" s="8" t="s">
         <v>120</v>
       </c>
@@ -2803,7 +2890,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2">
       <c r="A131" s="8" t="s">
         <v>232</v>
       </c>
@@ -2811,7 +2898,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2">
       <c r="A132" s="8" t="s">
         <v>109</v>
       </c>
@@ -2819,7 +2906,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2">
       <c r="A133" s="8" t="s">
         <v>233</v>
       </c>
@@ -2827,7 +2914,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2">
       <c r="A134" s="8" t="s">
         <v>109</v>
       </c>
@@ -2835,7 +2922,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2">
       <c r="A135" s="8" t="s">
         <v>234</v>
       </c>
@@ -2843,7 +2930,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2">
       <c r="A136" s="8" t="s">
         <v>109</v>
       </c>
@@ -2851,7 +2938,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2">
       <c r="A137" s="8" t="s">
         <v>236</v>
       </c>
@@ -2859,7 +2946,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2">
       <c r="A138" s="8" t="s">
         <v>236</v>
       </c>
@@ -2867,7 +2954,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2">
       <c r="A139" s="8" t="s">
         <v>109</v>
       </c>
@@ -2875,7 +2962,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2">
       <c r="A140" s="8" t="s">
         <v>109</v>
       </c>
@@ -2883,7 +2970,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2">
       <c r="A141" s="8" t="s">
         <v>109</v>
       </c>
@@ -2891,7 +2978,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2">
       <c r="A142" s="8" t="s">
         <v>109</v>
       </c>
@@ -2899,7 +2986,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2">
       <c r="A143" s="8" t="s">
         <v>117</v>
       </c>
@@ -2907,7 +2994,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2">
       <c r="A144" s="8" t="s">
         <v>195</v>
       </c>
@@ -2915,7 +3002,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2">
       <c r="A145" s="8" t="s">
         <v>117</v>
       </c>
@@ -2923,7 +3010,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2">
       <c r="A146" s="8" t="s">
         <v>117</v>
       </c>
@@ -2931,7 +3018,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2">
       <c r="A147" s="8" t="s">
         <v>117</v>
       </c>
@@ -2939,7 +3026,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2">
       <c r="A148" s="8" t="s">
         <v>109</v>
       </c>
@@ -2958,48 +3045,1253 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DCA210-A6D3-4735-B8FE-1EE9D3A9F662}">
+  <dimension ref="A1:B148"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="54.75" customHeight="1">
+      <c r="A1" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B1" s="12"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46FF3F35-4910-4014-B8BC-19956207C766}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" customWidth="1"/>
-    <col min="3" max="3" width="45.33203125" customWidth="1"/>
-    <col min="5" max="5" width="22.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="45.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:3" ht="66" customHeight="1">
+      <c r="A1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="11"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:3" ht="16.149999999999999" customHeight="1">
+      <c r="A3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="14" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="13" t="s">
         <v>15</v>
       </c>
@@ -3008,7 +4300,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
@@ -3017,7 +4309,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="13" t="s">
         <v>2</v>
       </c>
@@ -3026,7 +4318,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="13" t="s">
         <v>3</v>
       </c>
@@ -3035,7 +4327,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="13" t="s">
         <v>8</v>
       </c>
@@ -3044,7 +4336,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="13" t="s">
         <v>1</v>
       </c>
@@ -3053,7 +4345,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" s="13" t="s">
         <v>14</v>
       </c>
@@ -3062,7 +4354,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="13" t="s">
         <v>0</v>
       </c>
@@ -3071,7 +4363,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" s="13" t="s">
         <v>12</v>
       </c>
@@ -3080,7 +4372,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="13" t="s">
         <v>10</v>
       </c>
@@ -3089,7 +4381,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="13" t="s">
         <v>13</v>
       </c>
@@ -3098,7 +4390,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="13" t="s">
         <v>18</v>
       </c>
@@ -3107,7 +4399,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" s="13" t="s">
         <v>11</v>
       </c>
@@ -3116,7 +4408,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" s="13" t="s">
         <v>9</v>
       </c>
@@ -3125,7 +4417,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" s="13" t="s">
         <v>16</v>
       </c>
@@ -3134,7 +4426,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" s="13" t="s">
         <v>5</v>
       </c>
@@ -3143,7 +4435,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" s="13" t="s">
         <v>36</v>
       </c>
@@ -3152,7 +4444,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" s="13" t="s">
         <v>61</v>
       </c>
@@ -3163,27 +4455,27 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Tercera pasada y cambios de sintaxis
</commit_message>
<xml_diff>
--- a/Quindim/Quindim Src.xlsx
+++ b/Quindim/Quindim Src.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITNL\7° Semestre - I.S.C\Leng. y Automat. 2\Lenguaje\Quindim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC9B05A-C9DF-4BC5-B413-014CCB219EA0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E297763-5562-4C3F-B204-FB8AD09BF0FC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{674D8D03-4B2E-43D7-B73B-FEE82AEA8288}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{674D8D03-4B2E-43D7-B73B-FEE82AEA8288}"/>
   </bookViews>
   <sheets>
     <sheet name="Lexicon" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="263">
   <si>
     <t>print</t>
   </si>
@@ -927,6 +927,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -935,9 +938,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1460,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE269D34-044F-4D77-B821-FA589F4C7EB1}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1835,6 +1835,14 @@
         <v>262</v>
       </c>
       <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="48" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C48" s="3"/>
@@ -3071,8 +3079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46FF3F35-4910-4014-B8BC-19956207C766}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3088,212 +3096,212 @@
       <c r="A1" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="14"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="15"/>
+      <c r="B3" s="16"/>
       <c r="C3" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="16"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="16"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="16"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="16"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="16"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="16"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="16"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="16"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="16"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="16"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="16"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="16"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="16"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="2" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>